<commit_message>
Water collection data bug
</commit_message>
<xml_diff>
--- a/videosExcel.xlsx
+++ b/videosExcel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="20260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="videos" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
           </cell>
         </row>
         <row r="33">
-          <cell r="AD33">
-            <v>4.2155329743505873E-3</v>
-          </cell>
           <cell r="AE33">
             <v>10.122404682274208</v>
           </cell>
@@ -259,9 +256,6 @@
           </cell>
         </row>
         <row r="34">
-          <cell r="AD34">
-            <v>4.422065171836481E-3</v>
-          </cell>
           <cell r="AE34">
             <v>10.118363015075275</v>
           </cell>
@@ -282,9 +276,6 @@
           </cell>
         </row>
         <row r="35">
-          <cell r="AD35">
-            <v>6.9253609178478344E-3</v>
-          </cell>
           <cell r="AE35">
             <v>10.126310975610028</v>
           </cell>
@@ -305,9 +296,6 @@
           </cell>
         </row>
         <row r="36">
-          <cell r="AD36">
-            <v>7.0122871945566007E-3</v>
-          </cell>
           <cell r="AE36">
             <v>10.122926963993399</v>
           </cell>
@@ -328,9 +316,6 @@
           </cell>
         </row>
         <row r="37">
-          <cell r="AD37">
-            <v>5.7492592644203065E-3</v>
-          </cell>
           <cell r="AE37">
             <v>10.111522123894652</v>
           </cell>
@@ -351,9 +336,6 @@
           </cell>
         </row>
         <row r="38">
-          <cell r="AD38">
-            <v>3.2385401505251373E-3</v>
-          </cell>
           <cell r="AE38">
             <v>10.27301580498275</v>
           </cell>
@@ -374,9 +356,6 @@
           </cell>
         </row>
         <row r="39">
-          <cell r="AD39">
-            <v>6.3672554396339946E-3</v>
-          </cell>
           <cell r="AE39">
             <v>10.070849447236048</v>
           </cell>
@@ -397,9 +376,6 @@
           </cell>
         </row>
         <row r="40">
-          <cell r="AD40">
-            <v>6.8138427152222777E-3</v>
-          </cell>
           <cell r="AE40">
             <v>10.132851727982203</v>
           </cell>
@@ -420,9 +396,6 @@
           </cell>
         </row>
         <row r="41">
-          <cell r="AD41">
-            <v>8.4729514288380478E-3</v>
-          </cell>
           <cell r="AE41">
             <v>10.10331869643494</v>
           </cell>
@@ -443,9 +416,6 @@
           </cell>
         </row>
         <row r="42">
-          <cell r="AD42">
-            <v>8.4209559639078849E-3</v>
-          </cell>
           <cell r="AE42">
             <v>10.103624622812271</v>
           </cell>
@@ -466,9 +436,6 @@
           </cell>
         </row>
         <row r="43">
-          <cell r="AD43">
-            <v>9.6700446265201526E-3</v>
-          </cell>
           <cell r="AE43">
             <v>10.117567559611773</v>
           </cell>
@@ -489,9 +456,6 @@
           </cell>
         </row>
         <row r="44">
-          <cell r="AD44">
-            <v>7.9516282933473174E-3</v>
-          </cell>
           <cell r="AE44">
             <v>10.10192687411597</v>
           </cell>
@@ -512,9 +476,6 @@
           </cell>
         </row>
         <row r="45">
-          <cell r="AD45">
-            <v>9.8232151758798902E-3</v>
-          </cell>
           <cell r="AE45">
             <v>10.096097067280533</v>
           </cell>
@@ -535,9 +496,6 @@
           </cell>
         </row>
         <row r="46">
-          <cell r="AD46">
-            <v>1.0000104660430336E-2</v>
-          </cell>
           <cell r="AE46">
             <v>10.103747901388381</v>
           </cell>
@@ -855,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -882,10 +840,9 @@
 ",A1,"-",B1,"
 Cooling Plate Temp (C): ",E1,"
 Chamber Temp: (C): ",F1,"
-Humidity (%RH): ",G1,"
-Water Collection Rate: ",H1
+Humidity (%RH): ",G1
 )</f>
-        <v>Bare Glass Sample (control)_x000D_180217-BG1-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 24.2 +/- 0.2_x000D_Humidity (%RH): 80.9 +/- 0.7_x000D_Water Collection Rate: 8.6E-03</v>
+        <v>Bare Glass Sample (control)_x000D_180217-BG1-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 24.2 +/- 0.2_x000D_Humidity (%RH): 80.9 +/- 0.7</v>
       </c>
       <c r="E1" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE32,1)," +/- ",ROUND([1]Data!AF32,1))</f>
@@ -899,15 +856,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI32,1)," +/- ",ROUND([1]Data!AJ32,1))</f>
         <v>80.9 +/- 0.7</v>
       </c>
-      <c r="H1" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD32*1000,1),"E-03")</f>
-        <v>8.6E-03</v>
-      </c>
       <c r="I1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -922,15 +875,9 @@
 ",A2,"-",B2,"
 Cooling Plate Temp (C): ",E2,"
 Chamber Temp: (C): ",F2,"
-Humidity (%RH): ",G2,"
-Water Collection Rate: ",H2
+Humidity (%RH): ",G2
 )</f>
-        <v>Bare Glass Sample (control)
-180217-BG1-T2
-Cooling Plate Temp (C): 10.1 +/- 0.3
-Chamber Temp: (C): 22.8 +/- 0
-Humidity (%RH): 90 +/- 0.2
-Water Collection Rate: 4.2E-03</v>
+        <v>Bare Glass Sample (control)_x000D_180217-BG1-T2_x000D_Cooling Plate Temp (C): 10.1 +/- 0.3_x000D_Chamber Temp: (C): 22.8 +/- 0_x000D_Humidity (%RH): 90 +/- 0.2</v>
       </c>
       <c r="E2" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE33,1)," +/- ",ROUND([1]Data!AF33,1))</f>
@@ -944,15 +891,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI33,1)," +/- ",ROUND([1]Data!AJ33,1))</f>
         <v>90 +/- 0.2</v>
       </c>
-      <c r="H2" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD33*1000,1),"E-03")</f>
-        <v>4.2E-03</v>
-      </c>
       <c r="I2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -964,12 +907,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hydrophobic Sample (control)
-180217-HO1-T1
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 22.7 +/- 0.2
-Humidity (%RH): 88.4 +/- 0.2
-Water Collection Rate: 4.4E-03</v>
+        <v>Hydrophobic Sample (control)_x000D_180217-HO1-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 22.7 +/- 0.2_x000D_Humidity (%RH): 88.4 +/- 0.2</v>
       </c>
       <c r="E3" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE34,1)," +/- ",ROUND([1]Data!AF34,1))</f>
@@ -983,15 +921,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI34,1)," +/- ",ROUND([1]Data!AJ34,1))</f>
         <v>88.4 +/- 0.2</v>
       </c>
-      <c r="H3" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD34*1000,1),"E-03")</f>
-        <v>4.4E-03</v>
-      </c>
       <c r="I3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1003,12 +937,7 @@
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hydrophobic Sample (control)
-180217-HO1-T2
-Cooling Plate Temp (C): 10.1 +/- 0.3
-Chamber Temp: (C): 23 +/- 0.3
-Humidity (%RH): 89.9 +/- 0.3
-Water Collection Rate: 6.9E-03</v>
+        <v>Hydrophobic Sample (control)_x000D_180217-HO1-T2_x000D_Cooling Plate Temp (C): 10.1 +/- 0.3_x000D_Chamber Temp: (C): 23 +/- 0.3_x000D_Humidity (%RH): 89.9 +/- 0.3</v>
       </c>
       <c r="E4" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE35,1)," +/- ",ROUND([1]Data!AF35,1))</f>
@@ -1022,15 +951,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI35,1)," +/- ",ROUND([1]Data!AJ35,1))</f>
         <v>89.9 +/- 0.3</v>
       </c>
-      <c r="H4" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD35*1000,1),"E-03")</f>
-        <v>6.9E-03</v>
-      </c>
       <c r="I4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1042,12 +967,7 @@
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hydrophobic Sample (control)
-180217-HO1-T3
-Cooling Plate Temp (C): 10.1 +/- 0.3
-Chamber Temp: (C): 23 +/- 0.4
-Humidity (%RH): 88.8 +/- 1.2
-Water Collection Rate: 7E-03</v>
+        <v>Hydrophobic Sample (control)_x000D_180217-HO1-T3_x000D_Cooling Plate Temp (C): 10.1 +/- 0.3_x000D_Chamber Temp: (C): 23 +/- 0.4_x000D_Humidity (%RH): 88.8 +/- 1.2</v>
       </c>
       <c r="E5" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE36,1)," +/- ",ROUND([1]Data!AF36,1))</f>
@@ -1061,15 +981,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI36,1)," +/- ",ROUND([1]Data!AJ36,1))</f>
         <v>88.8 +/- 1.2</v>
       </c>
-      <c r="H5" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD36*1000,1),"E-03")</f>
-        <v>7E-03</v>
-      </c>
       <c r="I5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1081,12 +997,7 @@
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Bare Glass Sample (control)
-180220-BG1-T1
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 23.1 +/- 0.2
-Humidity (%RH): 91.9 +/- 0.4
-Water Collection Rate: 5.7E-03</v>
+        <v>Bare Glass Sample (control)_x000D_180220-BG1-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 23.1 +/- 0.2_x000D_Humidity (%RH): 91.9 +/- 0.4</v>
       </c>
       <c r="E6" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE37,1)," +/- ",ROUND([1]Data!AF37,1))</f>
@@ -1100,15 +1011,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI37,1)," +/- ",ROUND([1]Data!AJ37,1))</f>
         <v>91.9 +/- 0.4</v>
       </c>
-      <c r="H6" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD37*1000,1),"E-03")</f>
-        <v>5.7E-03</v>
-      </c>
       <c r="I6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1120,12 +1027,7 @@
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top
-180221-HS1mm4mm2row-T1
-Cooling Plate Temp (C): 10.3 +/- 0.7
-Chamber Temp: (C): 22.9 +/- 0.7
-Humidity (%RH): 89.6 +/- 0.4
-Water Collection Rate: 3.2E-03</v>
+        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top_x000D_180221-HS1mm4mm2row-T1_x000D_Cooling Plate Temp (C): 10.3 +/- 0.7_x000D_Chamber Temp: (C): 22.9 +/- 0.7_x000D_Humidity (%RH): 89.6 +/- 0.4</v>
       </c>
       <c r="E7" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE38,1)," +/- ",ROUND([1]Data!AF38,1))</f>
@@ -1139,15 +1041,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI38,1)," +/- ",ROUND([1]Data!AJ38,1))</f>
         <v>89.6 +/- 0.4</v>
       </c>
-      <c r="H7" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD38*1000,1),"E-03")</f>
-        <v>3.2E-03</v>
-      </c>
       <c r="I7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1159,12 +1057,7 @@
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top
-180221-HS1mm4mm2row-T2
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 22.9 +/- 0.7
-Humidity (%RH): 91.5 +/- 0.3
-Water Collection Rate: 6.4E-03</v>
+        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top_x000D_180221-HS1mm4mm2row-T2_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 22.9 +/- 0.7_x000D_Humidity (%RH): 91.5 +/- 0.3</v>
       </c>
       <c r="E8" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE39,1)," +/- ",ROUND([1]Data!AF39,1))</f>
@@ -1178,15 +1071,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI39,1)," +/- ",ROUND([1]Data!AJ39,1))</f>
         <v>91.5 +/- 0.3</v>
       </c>
-      <c r="H8" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD39*1000,1),"E-03")</f>
-        <v>6.4E-03</v>
-      </c>
       <c r="I8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1198,12 +1087,7 @@
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top
-180221-HS1mm4mm2row-T3
-Cooling Plate Temp (C): 10.1 +/- 0.3
-Chamber Temp: (C): 23.7 +/- 0.3
-Humidity (%RH): 90.9 +/- 0.3
-Water Collection Rate: 6.8E-03</v>
+        <v>Hybrid surface- 1mm features - 4mm distance - 2 rows on top_x000D_180221-HS1mm4mm2row-T3_x000D_Cooling Plate Temp (C): 10.1 +/- 0.3_x000D_Chamber Temp: (C): 23.7 +/- 0.3_x000D_Humidity (%RH): 90.9 +/- 0.3</v>
       </c>
       <c r="E9" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE40,1)," +/- ",ROUND([1]Data!AF40,1))</f>
@@ -1217,15 +1101,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI40,1)," +/- ",ROUND([1]Data!AJ40,1))</f>
         <v>90.9 +/- 0.3</v>
       </c>
-      <c r="H9" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD40*1000,1),"E-03")</f>
-        <v>6.8E-03</v>
-      </c>
       <c r="I9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1237,12 +1117,7 @@
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top
-180222-HS2mm4mm2row-T1
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 24.1 +/- 0.3
-Humidity (%RH): 90.1 +/- 0.4
-Water Collection Rate: 8.5E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top_x000D_180222-HS2mm4mm2row-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 24.1 +/- 0.3_x000D_Humidity (%RH): 90.1 +/- 0.4</v>
       </c>
       <c r="E10" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE41,1)," +/- ",ROUND([1]Data!AF41,1))</f>
@@ -1256,15 +1131,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI41,1)," +/- ",ROUND([1]Data!AJ41,1))</f>
         <v>90.1 +/- 0.4</v>
       </c>
-      <c r="H10" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD41*1000,1),"E-03")</f>
-        <v>8.5E-03</v>
-      </c>
       <c r="I10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1276,12 +1147,7 @@
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top
-180222-HS2mm4mm2row-T2
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 23.5 +/- 0.3
-Humidity (%RH): 90.1 +/- 0.3
-Water Collection Rate: 8.4E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top_x000D_180222-HS2mm4mm2row-T2_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 23.5 +/- 0.3_x000D_Humidity (%RH): 90.1 +/- 0.3</v>
       </c>
       <c r="E11" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE42,1)," +/- ",ROUND([1]Data!AF42,1))</f>
@@ -1295,15 +1161,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI42,1)," +/- ",ROUND([1]Data!AJ42,1))</f>
         <v>90.1 +/- 0.3</v>
       </c>
-      <c r="H11" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD42*1000,1),"E-03")</f>
-        <v>8.4E-03</v>
-      </c>
       <c r="I11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1315,12 +1177,7 @@
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top
-180222-HS2mm4mm2row-T3
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 24.1 +/- 0.3
-Humidity (%RH): 89.5 +/- 0.3
-Water Collection Rate: 9.7E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows on top_x000D_180222-HS2mm4mm2row-T3_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 24.1 +/- 0.3_x000D_Humidity (%RH): 89.5 +/- 0.3</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE43,1)," +/- ",ROUND([1]Data!AF43,1))</f>
@@ -1334,15 +1191,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI43,1)," +/- ",ROUND([1]Data!AJ43,1))</f>
         <v>89.5 +/- 0.3</v>
       </c>
-      <c r="H12" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD43*1000,1),"E-03")</f>
-        <v>9.7E-03</v>
-      </c>
       <c r="I12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="96" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1354,12 +1207,7 @@
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Bare Glass Sample (control)
-180225-BG3-T1
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 23.9 +/- 0.3
-Humidity (%RH): 89.4 +/- 0.4
-Water Collection Rate: 8E-03</v>
+        <v>Bare Glass Sample (control)_x000D_180225-BG3-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 23.9 +/- 0.3_x000D_Humidity (%RH): 89.4 +/- 0.4</v>
       </c>
       <c r="E13" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE44,1)," +/- ",ROUND([1]Data!AF44,1))</f>
@@ -1373,15 +1221,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI44,1)," +/- ",ROUND([1]Data!AJ44,1))</f>
         <v>89.4 +/- 0.4</v>
       </c>
-      <c r="H13" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD44*1000,1),"E-03")</f>
-        <v>8E-03</v>
-      </c>
       <c r="I13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1393,12 +1237,7 @@
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle
-180227-HS2mm4mm2row-mid-T1
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 24.1 +/- 0.3
-Humidity (%RH): 89.6 +/- 0.3
-Water Collection Rate: 9.8E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle_x000D_180227-HS2mm4mm2row-mid-T1_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 24.1 +/- 0.3_x000D_Humidity (%RH): 89.6 +/- 0.3</v>
       </c>
       <c r="E14" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE45,1)," +/- ",ROUND([1]Data!AF45,1))</f>
@@ -1412,15 +1251,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI45,1)," +/- ",ROUND([1]Data!AJ45,1))</f>
         <v>89.6 +/- 0.3</v>
       </c>
-      <c r="H14" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD45*1000,1),"E-03")</f>
-        <v>9.8E-03</v>
-      </c>
       <c r="I14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1432,12 +1267,7 @@
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle
-180227-HS2mm4mm2row-mid-T2
-Cooling Plate Temp (C): 10.1 +/- 0.2
-Chamber Temp: (C): 22.8 +/- 0.5
-Humidity (%RH): 90.4 +/- 0.5
-Water Collection Rate: 10E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle_x000D_180227-HS2mm4mm2row-mid-T2_x000D_Cooling Plate Temp (C): 10.1 +/- 0.2_x000D_Chamber Temp: (C): 22.8 +/- 0.5_x000D_Humidity (%RH): 90.4 +/- 0.5</v>
       </c>
       <c r="E15" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE46,1)," +/- ",ROUND([1]Data!AF46,1))</f>
@@ -1451,15 +1281,11 @@
         <f>_xlfn.CONCAT(ROUND([1]Data!AI46,1)," +/- ",ROUND([1]Data!AJ46,1))</f>
         <v>90.4 +/- 0.5</v>
       </c>
-      <c r="H15" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD46*1000,1),"E-03")</f>
-        <v>10E-03</v>
-      </c>
       <c r="I15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1471,12 +1297,7 @@
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle
-180227-HS2mm4mm2row-mid-T3
-Cooling Plate Temp (C): 0 +/- 0
-Chamber Temp: (C): 0 +/- 0
-Humidity (%RH): 0 +/- 0
-Water Collection Rate: 0E-03</v>
+        <v>Hybrid surface- 2mm features - 4mm distance - 2 rows in the middle_x000D_180227-HS2mm4mm2row-mid-T3_x000D_Cooling Plate Temp (C): 0 +/- 0_x000D_Chamber Temp: (C): 0 +/- 0_x000D_Humidity (%RH): 0 +/- 0</v>
       </c>
       <c r="E16" s="1" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AE47,1)," +/- ",ROUND([1]Data!AF47,1))</f>
@@ -1489,10 +1310,6 @@
       <c r="G16" t="str">
         <f>_xlfn.CONCAT(ROUND([1]Data!AI47,1)," +/- ",ROUND([1]Data!AJ47,1))</f>
         <v>0 +/- 0</v>
-      </c>
-      <c r="H16" t="str">
-        <f>_xlfn.CONCAT(ROUND([1]Data!AD47*1000,1),"E-03")</f>
-        <v>0E-03</v>
       </c>
       <c r="I16" t="s">
         <v>30</v>

</xml_diff>